<commit_message>
JIRA:101 - adding drools decision table - add business rules in decision table
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/order-rules.xlsx
+++ b/src/main/resources/rules/order-rules.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{4588F970-DCE2-48BF-B470-C6C64793581B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\business-rules-git\src\main\resources\rules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C828C994-6F06-48AE-96C6-B130CD77C2EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="20760" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="customer-rules" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -53,9 +57,6 @@
     <t>Payment is for physical product</t>
   </si>
   <si>
-    <t>"generate a packing slip"</t>
-  </si>
-  <si>
     <t>Payment is for book</t>
   </si>
   <si>
@@ -80,15 +81,6 @@
     <t>"UPG_MEMBERSHIP"</t>
   </si>
   <si>
-    <t>"b"</t>
-  </si>
-  <si>
-    <t>"m"</t>
-  </si>
-  <si>
-    <t>"u"</t>
-  </si>
-  <si>
     <t>Payment is for upgrde membership</t>
   </si>
   <si>
@@ -104,12 +96,6 @@
     <t>"VIDEO"</t>
   </si>
   <si>
-    <t>"video"</t>
-  </si>
-  <si>
-    <t>"m ug"</t>
-  </si>
-  <si>
     <t>"LEARNING_TO_SKI"</t>
   </si>
   <si>
@@ -119,20 +105,38 @@
     <t>"PHYPRD", "BOOK"</t>
   </si>
   <si>
-    <t>"phy book"</t>
-  </si>
-  <si>
     <t>attrName == $1</t>
-  </si>
-  <si>
-    <t>System.out.println("Output : " + $1 );
-orderOutput.setOutput(orderOutput.getOutput() +  " ," +$1);</t>
   </si>
   <si>
     <t xml:space="preserve">com.ani.drools.decision.demo.model.OrderRequest,
 com.ani.drools.decision.demo.model.PaymentType,
 com.ani.drools.decision.demo.model.OrderOutput
 </t>
+  </si>
+  <si>
+    <t>System.out.println("Output : " + $1 );
+orderOutput.setOutput(orderOutput.getOutput()  +$1);</t>
+  </si>
+  <si>
+    <t>"generate a packing slip for shipping"</t>
+  </si>
+  <si>
+    <t>"activate that membership"</t>
+  </si>
+  <si>
+    <t>"create a duplicate packing slip for the royalty department"</t>
+  </si>
+  <si>
+    <t>"apply the upgrade"</t>
+  </si>
+  <si>
+    <t>"add a free “First Aid” video to the packing slip"</t>
+  </si>
+  <si>
+    <t>"generate a commission payment to the agent"</t>
+  </si>
+  <si>
+    <t>"e-mail the owner and inform them of the activation/upgrade"</t>
   </si>
 </sst>
 </file>
@@ -569,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -578,7 +582,7 @@
     <col min="1" max="1" width="31.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.625" style="1" customWidth="1"/>
     <col min="3" max="4" width="41.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="50.25" style="1" customWidth="1"/>
+    <col min="5" max="5" width="164.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -598,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -648,18 +652,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="125.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -670,79 +674,79 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JIRA:101 - adding drools decision table - defect fix business rules
</commit_message>
<xml_diff>
--- a/src/main/resources/rules/order-rules.xlsx
+++ b/src/main/resources/rules/order-rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\business-rules-git\src\main\resources\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C828C994-6F06-48AE-96C6-B130CD77C2EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED35C5F-BA11-43E3-A6DE-25411D0347EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,29 +114,29 @@
 </t>
   </si>
   <si>
+    <t>"generate a packing slip for shipping"</t>
+  </si>
+  <si>
+    <t>"activate that membership"</t>
+  </si>
+  <si>
+    <t>"create a duplicate packing slip for the royalty department"</t>
+  </si>
+  <si>
+    <t>"apply the upgrade"</t>
+  </si>
+  <si>
+    <t>"add a free “First Aid” video to the packing slip"</t>
+  </si>
+  <si>
+    <t>"generate a commission payment to the agent"</t>
+  </si>
+  <si>
+    <t>"e-mail the owner and inform them of the activation/upgrade"</t>
+  </si>
+  <si>
     <t>System.out.println("Output : " + $1 );
-orderOutput.setOutput(orderOutput.getOutput()  +$1);</t>
-  </si>
-  <si>
-    <t>"generate a packing slip for shipping"</t>
-  </si>
-  <si>
-    <t>"activate that membership"</t>
-  </si>
-  <si>
-    <t>"create a duplicate packing slip for the royalty department"</t>
-  </si>
-  <si>
-    <t>"apply the upgrade"</t>
-  </si>
-  <si>
-    <t>"add a free “First Aid” video to the packing slip"</t>
-  </si>
-  <si>
-    <t>"generate a commission payment to the agent"</t>
-  </si>
-  <si>
-    <t>"e-mail the owner and inform them of the activation/upgrade"</t>
+orderOutput.setOutput( (orderOutput.getOutput()  != null &amp;&amp; !orderOutput.getOutput().trim() .equals("") )  ? orderOutput.getOutput() +  " ," +$1 : $1);</t>
   </si>
 </sst>
 </file>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -663,7 +663,7 @@
         <v>14</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -677,7 +677,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -688,7 +688,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -699,7 +699,7 @@
         <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -710,7 +710,7 @@
         <v>18</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -721,7 +721,7 @@
         <v>21</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>24</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -746,7 +746,7 @@
         <v>26</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>